<commit_message>
[CAN2-21] Config Reg Reqs
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/config_reg_requirements_eric.xlsx
+++ b/Life_Cycle_Data/config_reg_requirements_eric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010371\Documents\Can Controller\Reqs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A276D05-7585-440D-8F15-A8A14527E9C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0234CBE2-8E9D-45A7-BCB6-76AB95BB29FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Requirement Header</t>
   </si>
@@ -55,18 +55,6 @@
     <t>The module shall set o_reg_error to logic high when a non-default vaule is written to a reserved bit.</t>
   </si>
   <si>
-    <t>REG_GEN_04</t>
-  </si>
-  <si>
-    <t>The module shall set o_interrupt to logic high when any bit within the interrupt status register is set to logic high and the the corrisponding bit in the interrupt enable register is set to logic high.</t>
-  </si>
-  <si>
-    <t>REG_GEN_05</t>
-  </si>
-  <si>
-    <t>The module shall set o_soft_reset to logic high for one clock cycle on the rising edge of i_sys_clk when i_reg_w_bus(31) is logic high and i_rs_vector(0) is logic high.</t>
-  </si>
-  <si>
     <t>Tx Registers</t>
   </si>
   <si>
@@ -91,15 +79,9 @@
     <t>REG_HPB_02</t>
   </si>
   <si>
-    <t>The module shall set o_hpb_r_en to logic high for one clock cycle on the rising edge of i_sys_clk when i_rs_vector(17) is logic high.</t>
-  </si>
-  <si>
     <t>REG_HPB_03</t>
   </si>
   <si>
-    <t>The module shall set o_hpb_full to logic high for one clock cycle on the rising edge of i_sys_clk when i_r_neg_w is logic low and i_rs_vector is equal to 0x20000.</t>
-  </si>
-  <si>
     <t>Mode Select Register</t>
   </si>
   <si>
@@ -283,9 +265,6 @@
     <t>REG_ST_01</t>
   </si>
   <si>
-    <t>The module shall set bit 20 within to internal status register to i_acfbsy on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_ST_02</t>
   </si>
   <si>
@@ -295,120 +274,63 @@
     <t>REG_ST_03</t>
   </si>
   <si>
-    <t>The module shall set bit 25 within to internal status register to i_errwrn on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_ST_04</t>
   </si>
   <si>
-    <t>The module shall set bit 26 within to internal status register to i_bbsy on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_ST_05</t>
   </si>
   <si>
-    <t>The module shall set bit 27 within to internal status register to i_bidle on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_ST_06</t>
   </si>
   <si>
-    <t>The module shall set bit 28 within to internal status register to i_normal on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_ST_07</t>
   </si>
   <si>
-    <t>The module shall set bit 29 within to internal status register to i_sleep on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_ST_08</t>
   </si>
   <si>
-    <t>The module shall set bit 30 within to internal status register to i_lback on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_ST_09</t>
   </si>
   <si>
-    <t>The module shall set bit 31 within to internal status register to i_config on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>Interrupt Registers</t>
   </si>
   <si>
     <t>REG_INT_01</t>
   </si>
   <si>
-    <t>The module shall set bit 20 within to internal interrupt status register to i_wakeup on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_02</t>
   </si>
   <si>
-    <t>The module shall set bit 21 within to internal interrupt status register to i_sleep on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_03</t>
   </si>
   <si>
-    <t>The module shall set bit 22 within to internal interrupt status register to i_bsoff on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_04</t>
   </si>
   <si>
-    <t>The module shall set bit 23 within to internal interrupt status register to i_error on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_05</t>
   </si>
   <si>
-    <t>The module shall set bit 24 within to internal interrupt status register to i_rxnemp on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_06</t>
   </si>
   <si>
-    <t>The module shall set bit 25 within to internal interrupt status register to i_rxoflw on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_07</t>
   </si>
   <si>
-    <t>The module shall set bit 26 within to internal interrupt status register to i_rxuflw on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_09</t>
   </si>
   <si>
-    <t>The module shall set bit 27 within to internal interrupt status register to i_rxok on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_10</t>
   </si>
   <si>
-    <t>The module shall set bit 28 within to internal interrupt status register to o_hpb_full on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_11</t>
   </si>
   <si>
-    <t>The module shall set bit 29 within to internal interrupt status register to i_tx_full on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_12</t>
   </si>
   <si>
-    <t>The module shall set bit 30 within to internal interrupt status register to i_txok on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>REG_INT_13</t>
   </si>
   <si>
-    <t>The module shall set bit 31 within to internal interrupt status register to i_arblst on the rising edge of i_sys_clk.</t>
-  </si>
-  <si>
     <t>Error Count Registers</t>
   </si>
   <si>
@@ -428,6 +350,117 @@
   </si>
   <si>
     <t>REG_TX_02</t>
+  </si>
+  <si>
+    <t>The module shall set bit 27 within the internal status register to i_bidle on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 28 within the internal status register to i_normal on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 29 within the internal status register to i_sleep on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 30 within the internal status register to i_lback on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 31 within the internal status register to i_config on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 20 within the internal status register to i_acfbsy on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 25 within the internal status register to i_errwrn on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 26 within the internal status register to i_bbsy on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall latch o_hpb_full to logic high for one clock cycle on the rising edge of i_sys_clk when i_rs_vector(17) is logic high.</t>
+  </si>
+  <si>
+    <t>The module shall set o_hpb_full to logic low when i_hpb_r_en is logic high.</t>
+  </si>
+  <si>
+    <t>REG_INT_08</t>
+  </si>
+  <si>
+    <t>The module shall set o_soft_reset to logic high for one clock cycle on the rising edge of i_sys_clk when bit 31 within the software reset register is logic high and i_rs_vector(0) is logic high.</t>
+  </si>
+  <si>
+    <t>The module shall set o_cen to logic high when when bit 30 within the software reset register is logic low and i_rs_vector(0) is logic high.</t>
+  </si>
+  <si>
+    <t>Reset Register</t>
+  </si>
+  <si>
+    <t>REG_RST_02</t>
+  </si>
+  <si>
+    <t>REG_RST_01</t>
+  </si>
+  <si>
+    <t>The module shall set bit 20 within the internal interrupt status register to i_wakeup and bit 20 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 22 within the internal interrupt status register to i_bsoff and bit 22 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 21 within the internal interrupt status register to i_sleep and bit 21 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 23 within the internal interrupt status register to i_error and bit 23 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 24 within the internal interrupt status register to i_rxnemp and bit 24 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 25 within the internal interrupt status register to i_rxoflw and bit 25 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 26 within the internal interrupt status register to i_rxuflw and bit 26 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 27 within the internal interrupt status register to i_rxok and bit 27 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 28 within the internal interrupt status register to o_hpb_full and bit 28 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 29 within the internal interrupt status register to i_tx_full and bit 29 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 30 within the internal interrupt status register to i_txok and bit 30 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set bit 31 within the internal interrupt status register to i_arblst and bit 31 within the internal interrput enable register on the rising edge of i_sys_clk.</t>
+  </si>
+  <si>
+    <t>The module shall set the bit within the internal interrupt status register to logic low when the corrisponding bit within the internal interrupt clear register is logic high.</t>
+  </si>
+  <si>
+    <t>REG_INT_14</t>
+  </si>
+  <si>
+    <t>The module shall set o_interrupt to logic high when any bit within the interrupt status register is logic high.</t>
+  </si>
+  <si>
+    <t>Register Read</t>
+  </si>
+  <si>
+    <t>Register write</t>
+  </si>
+  <si>
+    <t>REG_RD_01</t>
+  </si>
+  <si>
+    <t>REG_WR_01</t>
+  </si>
+  <si>
+    <t>The module shall set o_reg_r_data to the connent of a register when the corrisponding bit within i_rs_vector is logic high and i_r_neg_w is logic high.</t>
+  </si>
+  <si>
+    <t>The module shall load i_reg_w_data into the a register when the corrisponding bit within i_rs_vector is logic high and i_r_neg_w is logic low.</t>
   </si>
 </sst>
 </file>
@@ -442,20 +475,26 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,7 +503,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,49 +568,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -583,7 +585,50 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,33 +636,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:J1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -844,11 +920,11 @@
     <col min="1" max="1" width="17.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="155.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="178" bestFit="1" customWidth="1"/>
     <col min="5" max="26" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,653 +934,696 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="14" t="s">
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="23"/>
+    </row>
+    <row r="18" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="7" t="s">
+    </row>
+    <row r="59" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="6" t="s">
+    </row>
+    <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
-      <c r="C61" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C61" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="4"/>
+      <c r="B64" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2425,22 +2544,27 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A2:A61"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B39:B47"/>
-    <mergeCell ref="B48:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B2:B6"/>
+  <mergeCells count="13">
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B41:B49"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B28"/>
-    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="B50:B63"/>
+    <mergeCell ref="A2:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>